<commit_message>
some item names are changed
</commit_message>
<xml_diff>
--- a/References.xlsx
+++ b/References.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhihuitang/repo/python/Provsvar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA16CDE-FF22-7D40-8759-3119A2E369C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA5FBC-0220-CF45-BE82-F44DCA5C8B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="680" windowWidth="28040" windowHeight="17440" xr2:uid="{DBE3080E-B9F2-3742-A561-42170D0095D6}"/>
+    <workbookView xWindow="38400" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{DBE3080E-B9F2-3742-A561-42170D0095D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Min</t>
   </si>
@@ -50,15 +50,9 @@
     <t>S-ACE (E/L)</t>
   </si>
   <si>
-    <t>B--Erytrocyter (10(12)/L)</t>
-  </si>
-  <si>
     <t>B--Hemoglobin (Hb) (g/L)</t>
   </si>
   <si>
-    <t>B--EVF ()</t>
-  </si>
-  <si>
     <t>P--25-OH Vitamin D2+D3 (nmol/L)</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>vB-Ca,fri ABL/PNA (mmol/L)</t>
   </si>
   <si>
-    <t>P--Kreatinin (enz) (umol/L)</t>
-  </si>
-  <si>
     <t>Pt-eGFR(Krea)relativ (mL/min/1.7)</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>P--Natrium (mmol/L)</t>
   </si>
   <si>
-    <t>P-Glukos (PNA) (mmol/L)</t>
-  </si>
-  <si>
     <t>vB-Glukos ABL/PNA (mmol/L)</t>
   </si>
   <si>
@@ -104,17 +92,41 @@
     <t>Pt-eGFR(CysC)relativ (mL/min/1.7)</t>
   </si>
   <si>
-    <t>B--Leukocyter (10(9)/L)</t>
-  </si>
-  <si>
     <t>B--MCV (fL)</t>
+  </si>
+  <si>
+    <t>B--Metamyelocyter (x10(9)/L)</t>
+  </si>
+  <si>
+    <t>B--Myelocyter (x10(9)/L)</t>
+  </si>
+  <si>
+    <t>B--EVF</t>
+  </si>
+  <si>
+    <t>P--Kreatinin (enz) (mikromol/L)</t>
+  </si>
+  <si>
+    <t>B--Leukocyter (x10(9)/L)</t>
+  </si>
+  <si>
+    <t>B--Erytrocyter (x10(12)/L)</t>
+  </si>
+  <si>
+    <t>P--Glukos (mmol/L)</t>
+  </si>
+  <si>
+    <t>B--Trombocyter (x10(9)/L)</t>
+  </si>
+  <si>
+    <t>B--Neutrofila granulocyter (x10(9)/L)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +135,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -138,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,14 +166,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37641AEF-A466-714D-B948-CFC59032FB63}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +546,7 @@
     <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -521,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -532,9 +568,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -543,9 +579,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>48</v>
@@ -554,9 +590,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>2.15</v>
@@ -565,7 +601,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -576,9 +612,9 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -587,9 +623,9 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -598,9 +634,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>80</v>
@@ -609,9 +645,9 @@
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -620,9 +656,9 @@
         <v>999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>1.6</v>
@@ -631,9 +667,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>0.7</v>
@@ -642,9 +678,9 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0.7</v>
@@ -653,9 +689,9 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>0.6</v>
@@ -664,9 +700,9 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>3.5</v>
@@ -675,9 +711,9 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>23</v>
+    <row r="16" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B16">
         <v>3.5</v>
@@ -685,10 +721,11 @@
       <c r="C16">
         <v>8.8000000000000007</v>
       </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>4.2</v>
@@ -699,7 +736,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18">
         <v>134</v>
@@ -710,7 +747,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>0.39</v>
@@ -721,7 +758,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>82</v>
@@ -732,12 +769,18 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>137</v>
+      </c>
+      <c r="C21">
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -748,13 +791,57 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
       <c r="C23">
         <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>145</v>
+      </c>
+      <c r="C24">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>1.6</v>
+      </c>
+      <c r="C25">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>-999</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>-999</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -763,12 +850,12 @@
       <formula>AND(ISNUMBER(B5),OR(B5&lt;2.15, B5&gt;2.5))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A23">
+  <conditionalFormatting sqref="A2:A27">
     <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="yesterday">
       <formula>FLOOR(A2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A23">
+  <conditionalFormatting sqref="A2:A27">
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rename to P--25-OH Vitamin D (nmol/L)
</commit_message>
<xml_diff>
--- a/References.xlsx
+++ b/References.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhihuitang/repo/python/Provsvar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA5FBC-0220-CF45-BE82-F44DCA5C8B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5EA410-EE60-464D-BE24-87948AE37721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{DBE3080E-B9F2-3742-A561-42170D0095D6}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>B--Hemoglobin (Hb) (g/L)</t>
   </si>
   <si>
-    <t>P--25-OH Vitamin D2+D3 (nmol/L)</t>
-  </si>
-  <si>
     <t>S-1,25-OH-Vitamin D (pmol/L)</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>B--Neutrofila granulocyter (x10(9)/L)</t>
+  </si>
+  <si>
+    <t>P--25-OH Vitamin D (nmol/L)</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,7 +570,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>48</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>2.15</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -625,7 +625,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>80</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>1.6</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.7</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0.7</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0.6</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>3.5</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="16" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>3.5</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>4.2</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0.39</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>82</v>
@@ -769,7 +769,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>137</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>145</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>1.6</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26">
         <v>-999</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27">
         <v>-999</v>

</xml_diff>